<commit_message>
Adding Error 2 and Error 3
</commit_message>
<xml_diff>
--- a/Troubleshooting-Data-Task/Copy of Error Troubleshooting Data Task.xlsx
+++ b/Troubleshooting-Data-Task/Copy of Error Troubleshooting Data Task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirja\Documents\Southbridge-Public-Schools-Tasks\Troubleshooting-Data-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A38D727-C7FD-4A81-9577-B54C0327A089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6383B417-64DC-4A3F-83A2-5607106E64CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -648,32 +648,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -695,7 +695,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -28799,8 +28799,8 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>